<commit_message>
Initial commit: added frontend and backend folders
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Expense" sheetId="1" r:id="rId1"/>
+    <sheet name="expense" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -398,14 +398,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Source</v>
+        <v>category</v>
       </c>
       <c r="B1" t="str">
         <v>Amount</v>
@@ -416,18 +416,40 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Food</v>
+        <v>Fun</v>
       </c>
       <c r="B2">
-        <v>250</v>
+        <v>10000</v>
       </c>
       <c r="C2" s="1">
-        <v>45748.66678240741</v>
+        <v>45801.22928240741</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Books</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45778.22928240741</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>food</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45717.22928240741</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>